<commit_message>
Allowing to define different intra-problem sets for each variable in the same equation: the model will generate as many equations as the linear combination of intra-problme sets of the variables of the symbolic equation. Filters on intra-problmes sets are working fine. Feature test added, working. This improves and generalize the solution of the GitHub issue #75 (multiple intra-problem sets).
</commit_message>
<xml_diff>
--- a/tests/models/features/multi_intra_sets/sets.xlsx
+++ b/tests/models/features/multi_intra_sets/sets.xlsx
@@ -1,41 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\models\features\multi_intra_sets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55F8DBD-62C5-4089-AD0D-4E61E16ECE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88292D33-72DC-44EB-9542-5F5DDF470858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2040" yWindow="2110" windowWidth="28800" windowHeight="15370" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="_set_products" sheetId="1" r:id="rId1"/>
-    <sheet name="_set_technologies" sheetId="2" r:id="rId2"/>
-    <sheet name="_set_years" sheetId="3" r:id="rId3"/>
+    <sheet name="_set_products" sheetId="7" r:id="rId1"/>
+    <sheet name="_set_technologies" sheetId="8" r:id="rId2"/>
+    <sheet name="_set_years" sheetId="9" r:id="rId3"/>
+    <sheet name="_set_hours" sheetId="6" r:id="rId4"/>
+    <sheet name="_set_scenarios" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>p_Names</t>
   </si>
@@ -43,28 +32,55 @@
     <t>t_Names</t>
   </si>
   <si>
+    <t>t_category</t>
+  </si>
+  <si>
     <t>y_Names</t>
   </si>
   <si>
+    <t>y_category</t>
+  </si>
+  <si>
+    <t>h_Names</t>
+  </si>
+  <si>
+    <t>s_Names</t>
+  </si>
+  <si>
+    <t>h1</t>
+  </si>
+  <si>
+    <t>h2</t>
+  </si>
+  <si>
+    <t>h3</t>
+  </si>
+  <si>
+    <t>h4</t>
+  </si>
+  <si>
+    <t>h5</t>
+  </si>
+  <si>
     <t>electricity</t>
   </si>
   <si>
     <t>heat</t>
   </si>
   <si>
-    <t>goods</t>
-  </si>
-  <si>
-    <t>power</t>
-  </si>
-  <si>
-    <t>boiler</t>
-  </si>
-  <si>
-    <t>industry</t>
-  </si>
-  <si>
-    <t>y_category</t>
+    <t>housing</t>
+  </si>
+  <si>
+    <t>detailed</t>
+  </si>
+  <si>
+    <t>transport</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>not-detailed</t>
   </si>
   <si>
     <t>warmup</t>
@@ -73,13 +89,13 @@
     <t>run</t>
   </si>
   <si>
-    <t>t_category</t>
-  </si>
-  <si>
-    <t>detailed</t>
-  </si>
-  <si>
-    <t>not-detailed</t>
+    <t>step</t>
+  </si>
+  <si>
+    <t>nze</t>
+  </si>
+  <si>
+    <t>opt</t>
   </si>
 </sst>
 </file>
@@ -441,11 +457,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A0088D-4C49-4C79-9B58-47EADB6A37BA}">
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -457,17 +473,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -476,45 +487,96 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E48CF471-6E31-45EA-844F-33EDA281ABBC}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.7265625" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE269985-3158-410A-BF21-CA5B4F65C1A5}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>6</v>
+      <c r="A2">
+        <v>2020</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
+      <c r="A3">
+        <v>2021</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>8</v>
+      <c r="A4">
+        <v>2022</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -522,70 +584,79 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B7"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE717790-A871-483D-9278-98E2EDCB2255}">
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>2025</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2026</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2027</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>2028</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>2029</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>2030</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>